<commit_message>
adding new cleaned species names
</commit_message>
<xml_diff>
--- a/data-processed/species_names_resolved_edited.xlsx
+++ b/data-processed/species_names_resolved_edited.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15700" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="760" windowWidth="28160" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="species_names_resolved" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="719">
   <si>
     <t>user_supplied_name</t>
   </si>
@@ -2507,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E647"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E280" sqref="E280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4537,7 +4537,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>166</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>167</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>168</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>169</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>170</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>171</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>172</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>173</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>174</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -4676,8 +4676,11 @@
       <c r="D154">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E154" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>177</v>
       </c>
@@ -4691,7 +4694,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>178</v>
       </c>
@@ -4705,7 +4708,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>179</v>
       </c>
@@ -4719,7 +4722,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>180</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>181</v>
       </c>
@@ -4747,7 +4750,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>182</v>
       </c>
@@ -5657,7 +5660,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>252</v>
       </c>
@@ -5670,8 +5673,11 @@
       <c r="D225">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E225" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>252</v>
       </c>
@@ -5684,8 +5690,11 @@
       <c r="D226">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E226" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>252</v>
       </c>
@@ -5699,7 +5708,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>256</v>
       </c>
@@ -5713,7 +5722,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>258</v>
       </c>
@@ -5727,7 +5736,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>259</v>
       </c>
@@ -5741,7 +5750,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>260</v>
       </c>
@@ -5755,7 +5764,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>261</v>
       </c>
@@ -5769,7 +5778,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>262</v>
       </c>
@@ -5783,7 +5792,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>263</v>
       </c>
@@ -5797,7 +5806,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>264</v>
       </c>
@@ -5811,7 +5820,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>265</v>
       </c>
@@ -5825,7 +5834,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>266</v>
       </c>
@@ -5839,7 +5848,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>267</v>
       </c>
@@ -5853,7 +5862,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>268</v>
       </c>
@@ -5867,7 +5876,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>269</v>
       </c>
@@ -6329,7 +6338,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>307</v>
       </c>
@@ -6343,7 +6352,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>308</v>
       </c>
@@ -6357,7 +6366,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>310</v>
       </c>
@@ -6371,7 +6380,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>311</v>
       </c>
@@ -6385,7 +6394,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>312</v>
       </c>
@@ -6399,7 +6408,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>313</v>
       </c>
@@ -6413,7 +6422,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>314</v>
       </c>
@@ -6427,7 +6436,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>314</v>
       </c>
@@ -6440,8 +6449,11 @@
       <c r="D280">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E280" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>317</v>
       </c>
@@ -6455,7 +6467,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>318</v>
       </c>
@@ -6469,7 +6481,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>319</v>
       </c>
@@ -6483,7 +6495,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>320</v>
       </c>
@@ -6497,7 +6509,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>321</v>
       </c>
@@ -6511,7 +6523,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>322</v>
       </c>
@@ -6525,7 +6537,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>323</v>
       </c>
@@ -6539,7 +6551,7 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>324</v>
       </c>

</xml_diff>